<commit_message>
DSA: 11th April 25
</commit_message>
<xml_diff>
--- a/Jobs list.xlsx
+++ b/Jobs list.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C46594B-F8A1-4F7E-80AD-0306821167BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85100C8-03AC-444A-B3F1-F6DBBF9326A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{66BC1706-30CD-4FA2-AABB-8CD086E33348}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{66BC1706-30CD-4FA2-AABB-8CD086E33348}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="148">
   <si>
     <t>Duetsche</t>
   </si>
@@ -138,24 +139,6 @@
     <t>R-236056</t>
   </si>
   <si>
-    <t>JR-0000022440</t>
-  </si>
-  <si>
-    <t>JR-0000030351</t>
-  </si>
-  <si>
-    <t>JR-0000034344</t>
-  </si>
-  <si>
-    <t>JR-0000033912</t>
-  </si>
-  <si>
-    <t>JR-0000032174</t>
-  </si>
-  <si>
-    <t>JR-0000032145</t>
-  </si>
-  <si>
     <t>305007BR</t>
   </si>
   <si>
@@ -177,22 +160,6 @@
     <t>R-240682</t>
   </si>
   <si>
-    <t>JR-0000030225</t>
-  </si>
-  <si>
-    <t>JR-0000014106</t>
-  </si>
-  <si>
-    <t>JR-0000034120</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JR-0000004828
-</t>
-  </si>
-  <si>
-    <t>JR-0000009115</t>
-  </si>
-  <si>
     <t>sejal.zambare@bny.com</t>
   </si>
   <si>
@@ -217,9 +184,6 @@
     <t>R0376804</t>
   </si>
   <si>
-    <t>JR-0000029492</t>
-  </si>
-  <si>
     <t>R-240686</t>
   </si>
   <si>
@@ -229,26 +193,6 @@
     <t>R-221309</t>
   </si>
   <si>
-    <t>JR-0000033960</t>
-  </si>
-  <si>
-    <t>JR-0000035247</t>
-  </si>
-  <si>
-    <t>JR-0000024266</t>
-  </si>
-  <si>
-    <t>JR-0000037999</t>
-  </si>
-  <si>
-    <t>JR-0000020335</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JR-0000020246
-JR-0000020327
-</t>
-  </si>
-  <si>
     <t>R-242413</t>
   </si>
   <si>
@@ -258,65 +202,290 @@
     <t>R-242691</t>
   </si>
   <si>
-    <t>R0377739</t>
-  </si>
-  <si>
-    <t>JR-0000032695</t>
-  </si>
-  <si>
-    <t>JR-0000032711</t>
-  </si>
-  <si>
-    <t>JR-0000031848</t>
-  </si>
-  <si>
-    <t>JR-0000031853</t>
-  </si>
-  <si>
-    <t>JR-0000031833</t>
-  </si>
-  <si>
-    <t>JR-0000038702</t>
-  </si>
-  <si>
-    <t>JR-0000032710</t>
-  </si>
-  <si>
-    <t>JR-0000036922</t>
-  </si>
-  <si>
-    <t>JR-0000002474</t>
-  </si>
-  <si>
-    <t>JR-0000020322</t>
-  </si>
-  <si>
-    <t>JR-0000038958</t>
-  </si>
-  <si>
-    <t>R-229310 </t>
-  </si>
-  <si>
-    <t>R-233891</t>
+    <t>R-044340</t>
+  </si>
+  <si>
+    <t>SAP Labs</t>
+  </si>
+  <si>
+    <t>R-245067</t>
+  </si>
+  <si>
+    <t>R-244431</t>
+  </si>
+  <si>
+    <t>R-243890</t>
   </si>
   <si>
     <t>R-240090</t>
   </si>
   <si>
-    <t>R-219288</t>
-  </si>
-  <si>
-    <t>R-044340</t>
-  </si>
-  <si>
-    <t>SAP Labs</t>
+    <t>JR-0000018286</t>
+  </si>
+  <si>
+    <t>JR-0000011513</t>
+  </si>
+  <si>
+    <t>JR-0000035657</t>
+  </si>
+  <si>
+    <t>JR-0000039277</t>
+  </si>
+  <si>
+    <t>JR-0000009044</t>
+  </si>
+  <si>
+    <t>JR-0000036568</t>
+  </si>
+  <si>
+    <t>JR-0000020808</t>
+  </si>
+  <si>
+    <t>JR-0000006932</t>
+  </si>
+  <si>
+    <t>JR-0000038052</t>
+  </si>
+  <si>
+    <t>Atlassian</t>
+  </si>
+  <si>
+    <t>Druva</t>
+  </si>
+  <si>
+    <t>PubMatic </t>
+  </si>
+  <si>
+    <t>Mindtickle</t>
+  </si>
+  <si>
+    <t>Rubrik</t>
+  </si>
+  <si>
+    <t>Veritas Technologies LLC</t>
+  </si>
+  <si>
+    <t>Thoughtworks</t>
+  </si>
+  <si>
+    <t>Sirion</t>
+  </si>
+  <si>
+    <t>BrowserStack</t>
+  </si>
+  <si>
+    <t>Birdeye</t>
+  </si>
+  <si>
+    <t>CrowdStrike</t>
+  </si>
+  <si>
+    <t>ServiceNow</t>
+  </si>
+  <si>
+    <t>Veeam Software</t>
+  </si>
+  <si>
+    <t>Deloitte</t>
+  </si>
+  <si>
+    <t>Accenture</t>
+  </si>
+  <si>
+    <t>Tech Mahindra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HCLTech </t>
+  </si>
+  <si>
+    <t>Concentrix</t>
+  </si>
+  <si>
+    <t>McKinsey &amp; Company</t>
+  </si>
+  <si>
+    <t>JPMorganChase</t>
+  </si>
+  <si>
+    <t>Morgan Stanley</t>
+  </si>
+  <si>
+    <t>Wells Fargo</t>
+  </si>
+  <si>
+    <t>Bank of America</t>
+  </si>
+  <si>
+    <t>Boston Consulting Group</t>
+  </si>
+  <si>
+    <t>Bain &amp; Company</t>
+  </si>
+  <si>
+    <t>BCG X</t>
+  </si>
+  <si>
+    <t>Kearney</t>
+  </si>
+  <si>
+    <t>Oliver Wyman</t>
+  </si>
+  <si>
+    <t>American Express</t>
+  </si>
+  <si>
+    <t>Visa</t>
+  </si>
+  <si>
+    <t>Meta</t>
+  </si>
+  <si>
+    <t>Salesforce</t>
+  </si>
+  <si>
+    <t>SAP</t>
+  </si>
+  <si>
+    <t>Cisco</t>
+  </si>
+  <si>
+    <t>NVIDIA</t>
+  </si>
+  <si>
+    <t>Dell Technologies</t>
+  </si>
+  <si>
+    <t>Intel Corporation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amazon Web Services (AWS) </t>
+  </si>
+  <si>
+    <t>Adobe</t>
+  </si>
+  <si>
+    <t>Intuit</t>
+  </si>
+  <si>
+    <t>LinkedIn</t>
+  </si>
+  <si>
+    <t>Airbnb</t>
+  </si>
+  <si>
+    <t>Spotify</t>
+  </si>
+  <si>
+    <t>Uber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Netflix </t>
+  </si>
+  <si>
+    <t>Mastercard</t>
+  </si>
+  <si>
+    <t>PayPal</t>
+  </si>
+  <si>
+    <t>Capital One</t>
+  </si>
+  <si>
+    <t>Deutsche Bank</t>
+  </si>
+  <si>
+    <t>BNP Paribas</t>
+  </si>
+  <si>
+    <t>BlackRock</t>
+  </si>
+  <si>
+    <t>Blackstone</t>
+  </si>
+  <si>
+    <t>Fidelity Investment</t>
+  </si>
+  <si>
+    <t>Nestlé</t>
+  </si>
+  <si>
+    <t>PepsiCo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Procter &amp; Gamble </t>
+  </si>
+  <si>
+    <t>Johnson &amp; Johnson</t>
+  </si>
+  <si>
+    <t>Mondelēz International</t>
+  </si>
+  <si>
+    <t>Ferrero</t>
+  </si>
+  <si>
+    <t>Myntra</t>
+  </si>
+  <si>
+    <t>Flipkart</t>
+  </si>
+  <si>
+    <t>Meesho</t>
+  </si>
+  <si>
+    <t>Nykaa</t>
+  </si>
+  <si>
+    <t>Zepto</t>
+  </si>
+  <si>
+    <t>Blinkit</t>
+  </si>
+  <si>
+    <t>PhonePe</t>
+  </si>
+  <si>
+    <t>Lenskart.com</t>
+  </si>
+  <si>
+    <t>Unilever</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
+    <t>Palo Alto Networks</t>
+  </si>
+  <si>
+    <t>Synechron</t>
+  </si>
+  <si>
+    <t>Birlasoft</t>
+  </si>
+  <si>
+    <t>YASH Technologies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Synchrony </t>
+  </si>
+  <si>
+    <t>Red Hat</t>
+  </si>
+  <si>
+    <t>Johnson Controls</t>
+  </si>
+  <si>
+    <t>R-208485</t>
+  </si>
+  <si>
+    <t>R-245349</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -367,21 +536,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF494949"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -398,24 +554,15 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
-      <color rgb="FF53565A"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Inherit"/>
     </font>
   </fonts>
   <fills count="4">
@@ -451,7 +598,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -462,33 +609,24 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -804,10 +942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DAE847-9658-4E2E-84C7-F096D2A61546}">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="C25" sqref="C25:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -815,6 +953,7 @@
     <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.21875" bestFit="1" customWidth="1"/>
@@ -852,13 +991,13 @@
         <v>25</v>
       </c>
       <c r="K1" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="L1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" t="s">
         <v>56</v>
-      </c>
-      <c r="M1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -871,8 +1010,8 @@
       <c r="C2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>34</v>
+      <c r="D2" s="7" t="s">
+        <v>61</v>
       </c>
       <c r="E2" s="5">
         <v>25827130</v>
@@ -881,7 +1020,7 @@
       <c r="G2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="16">
+      <c r="H2" s="13">
         <v>266604</v>
       </c>
       <c r="I2" s="8" t="s">
@@ -890,13 +1029,13 @@
       <c r="J2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="L2" s="13">
+      <c r="K2" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" s="10">
         <v>28496</v>
       </c>
-      <c r="M2" s="26">
+      <c r="M2" s="17">
         <v>414830</v>
       </c>
     </row>
@@ -910,8 +1049,8 @@
       <c r="C3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>35</v>
+      <c r="D3" s="8">
+        <v>90391446</v>
       </c>
       <c r="E3" s="5">
         <v>25829520</v>
@@ -920,13 +1059,13 @@
       <c r="G3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="13">
         <v>266461</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="K3" s="12"/>
+        <v>42</v>
+      </c>
+      <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="2" t="s">
@@ -938,8 +1077,8 @@
       <c r="C4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>36</v>
+      <c r="D4" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="E4" s="5">
         <v>25827137</v>
@@ -947,29 +1086,31 @@
       <c r="G4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="13">
         <v>273102</v>
       </c>
-      <c r="K4" s="12"/>
+      <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="19"/>
+      <c r="B5" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="C5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>37</v>
+      <c r="D5" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="E5" s="5">
         <v>25827135</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="16">
+        <v>34</v>
+      </c>
+      <c r="H5" s="13">
         <v>269037</v>
       </c>
     </row>
@@ -977,187 +1118,140 @@
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="19" t="s">
-        <v>89</v>
-      </c>
       <c r="C6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="5">
-        <v>25827139</v>
+      <c r="D6" s="7" t="s">
+        <v>64</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" s="16">
+        <v>35</v>
+      </c>
+      <c r="H6" s="13">
         <v>273171</v>
       </c>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="5">
-        <v>25824475</v>
-      </c>
+      <c r="D7" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="9"/>
       <c r="G7" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="16">
+        <v>36</v>
+      </c>
+      <c r="H7" s="13">
         <v>266465</v>
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="5">
-        <v>25827533</v>
-      </c>
+      <c r="E8" s="9"/>
       <c r="G8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H8" s="13">
         <v>258938</v>
       </c>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="14" t="s">
-        <v>43</v>
+      <c r="A9" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="H9" s="13">
+        <v>258967</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10" s="16"/>
+      <c r="H10" s="13">
+        <v>283918</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="13">
+        <v>263186</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="5">
-        <v>25827539</v>
-      </c>
-      <c r="H9" s="16">
-        <v>258967</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="5">
-        <v>25827124</v>
-      </c>
-      <c r="G10" s="22"/>
-      <c r="H10" s="16">
-        <v>283918</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="28.2">
-      <c r="A11" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="5">
-        <v>24817184</v>
-      </c>
-      <c r="H11" s="16">
-        <v>263186</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="14" t="s">
-        <v>59</v>
-      </c>
       <c r="C12" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="5">
-        <v>25827471</v>
-      </c>
-      <c r="H12" s="16">
+        <v>39</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" s="13">
         <v>283934</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="C13" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="5">
-        <v>25829125</v>
-      </c>
-      <c r="H13" s="16">
+        <v>40</v>
+      </c>
+      <c r="H13" s="13">
         <v>284382</v>
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="E14" s="5">
-        <v>25836882</v>
+      <c r="A14" s="14"/>
+      <c r="C14" s="12" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="C15" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" s="5">
-        <v>25836886</v>
+        <v>50</v>
+      </c>
+      <c r="H15" s="18">
+        <v>276991</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="C16" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" s="5">
-        <v>25827958</v>
+        <v>51</v>
+      </c>
+      <c r="H16" s="18">
+        <v>286568</v>
       </c>
     </row>
     <row r="17" spans="3:6">
       <c r="C17" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E17" s="5">
-        <v>25836883</v>
+        <v>52</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>15</v>
@@ -1165,120 +1259,57 @@
     </row>
     <row r="18" spans="3:6">
       <c r="C18" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="E18" s="8">
-        <v>25829125</v>
+        <v>53</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="3:6">
       <c r="C19" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" s="5">
-        <v>25840732</v>
-      </c>
-    </row>
-    <row r="20" spans="3:6" ht="43.2">
-      <c r="D20" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" s="5">
-        <v>25825519</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6">
+      <c r="C20" s="19" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="3:6">
-      <c r="C21" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="E21" s="5">
-        <v>25842188</v>
+      <c r="C21" s="19" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="3:6">
-      <c r="C22" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="E22" s="5">
-        <v>25831516</v>
+      <c r="C22" s="19" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="3:6">
-      <c r="C23" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="D23" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="E23" s="23">
-        <v>25843205</v>
-      </c>
-    </row>
-    <row r="24" spans="3:6">
-      <c r="C24" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="D24" s="18" t="s">
-        <v>75</v>
+      <c r="C23" s="19" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="3:6">
-      <c r="C25" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="D25" s="21" t="s">
-        <v>76</v>
-      </c>
+      <c r="C25" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="F25" s="9"/>
     </row>
     <row r="26" spans="3:6">
-      <c r="D26" s="21" t="s">
-        <v>77</v>
+      <c r="C26" s="15" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="3:6">
-      <c r="D27" s="21" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="3:6">
-      <c r="D28" s="21" t="s">
-        <v>67</v>
-      </c>
+      <c r="C27" s="15"/>
     </row>
     <row r="29" spans="3:6">
-      <c r="D29" s="21" t="s">
-        <v>81</v>
-      </c>
+      <c r="C29" s="15"/>
+      <c r="E29" s="15"/>
     </row>
     <row r="30" spans="3:6">
-      <c r="D30" s="19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="3:6">
-      <c r="D31" s="19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="32" spans="3:6">
-      <c r="D32" s="19" t="s">
-        <v>84</v>
-      </c>
+      <c r="C30" s="15"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1288,4 +1319,432 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{289B9E9E-26DF-47B4-B63A-D3E664137F9D}">
+  <dimension ref="A2:A84"/>
+  <sheetViews>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="24.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>